<commit_message>
acho q ta bom
</commit_message>
<xml_diff>
--- a/resources/coleta.xlsx
+++ b/resources/coleta.xlsx
@@ -574,7 +574,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CPA ARMAZENS</t>
+          <t>SICOOB MERIDIONAL</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -595,7 +595,7 @@
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>ID_A-3369</t>
+          <t>ID_A-3370</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -611,11 +611,7 @@
       <c r="K3" t="n">
         <v>1</v>
       </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>COLETADO IA</t>
-        </is>
-      </c>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr">
         <is>
           <t>Sicoob_Meridional_PA_19_Blume_Janeiro_2025_Cód_441_ID_A-1962_</t>
@@ -635,7 +631,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CPA ARMAZENS</t>
+          <t>SICOOB MERIDIONAL</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -656,7 +652,7 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>ID_A-3369</t>
+          <t>ID_A-3371</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -672,11 +668,7 @@
       <c r="K4" t="n">
         <v>10</v>
       </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>COLETADO IA</t>
-        </is>
-      </c>
+      <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr">
         <is>
           <t>Sicoob_Meridional_Blume_Janeiro_2025_Cód_72_ID_A-1900_</t>

</xml_diff>